<commit_message>
ENH adding in new papers using AULS
</commit_message>
<xml_diff>
--- a/Papers/Published_AUL_papers.xlsx
+++ b/Papers/Published_AUL_papers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahalford/Documents/research/Collaborative_Programs/AUL/Papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E48C55B-A60B-3749-A782-13094A24E4E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE2426D-ED00-2E45-9F57-B4CC27B6B3DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7460" yWindow="2700" windowWidth="28040" windowHeight="17440" xr2:uid="{DD15ACF7-D5A3-5F45-ADEC-DF039DDAA86A}"/>
+    <workbookView xWindow="5560" yWindow="1960" windowWidth="28040" windowHeight="17440" xr2:uid="{DD15ACF7-D5A3-5F45-ADEC-DF039DDAA86A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>First Author</t>
   </si>
@@ -109,6 +109,32 @@
   </si>
   <si>
     <t>https://doi.org/10.1051/swsc/2019031</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s11214-020-00771-x</t>
+  </si>
+  <si>
+    <t>A Primer on Focused Solar Energetic Particle Transport
+Basic Physics and Recent Modelling Results</t>
+  </si>
+  <si>
+    <t>van den Berg</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s11214-020-00771-x</t>
+  </si>
+  <si>
+    <t>https://www.swsc-journal.org/articles/swsc/full_html/2020/01/swsc200079/swsc200079.html</t>
+  </si>
+  <si>
+    <t>The soft X-ray Neupert effect as a proxy for solar energetic particle injection
+A proof-of-concept physics-based forecasting model</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1051/swsc/2020067</t>
+  </si>
+  <si>
+    <t>Steyn</t>
   </si>
 </sst>
 </file>
@@ -476,13 +502,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBDD837-227A-144C-BF9A-E5028132B132}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="11" ySplit="20" topLeftCell="L21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,6 +622,40 @@
         <v>2019</v>
       </c>
     </row>
+    <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2020</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{02613E18-CF6A-654A-8B39-DF0CF8A4F5E4}"/>
@@ -608,6 +668,10 @@
     <hyperlink ref="D5" r:id="rId8" xr:uid="{584D0AF0-024F-674B-AC41-560764556E0F}"/>
     <hyperlink ref="C6" r:id="rId9" xr:uid="{8F855647-AF93-384F-B595-02CC9989C5F3}"/>
     <hyperlink ref="D6" r:id="rId10" xr:uid="{3DE9E024-C51F-4342-8B3E-F7AF82607794}"/>
+    <hyperlink ref="D7" r:id="rId11" xr:uid="{7FC1CB2E-EDCC-7E42-947E-0A398E223C40}"/>
+    <hyperlink ref="C7" r:id="rId12" xr:uid="{68ADC020-271E-FD43-8708-77C00C03E8E7}"/>
+    <hyperlink ref="C8" r:id="rId13" xr:uid="{9FE8DF70-99CE-3043-8A4F-D3A7A7FC4D32}"/>
+    <hyperlink ref="D8" r:id="rId14" xr:uid="{270DF36B-D2CA-4844-BA55-026FF669B9E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>